<commit_message>
update declare Negative Scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
+++ b/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.afify\IdeaProjects\vls-frontend-automation\src\test\resources\TestDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42CA8E4-DC61-40E2-B597-A3A453A112C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA52DAE-BD93-4C47-BF94-3F5452346DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewVehicleDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="declareVehicleDetails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="66">
   <si>
     <t>Persona_No</t>
   </si>
@@ -90,15 +91,9 @@
     <t xml:space="preserve">mortgageStatus </t>
   </si>
   <si>
-    <t>Insurance Period</t>
-  </si>
-  <si>
     <t>13</t>
   </si>
   <si>
-    <t>license Period</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
@@ -106,13 +101,136 @@
   </si>
   <si>
     <t>toRun</t>
+  </si>
+  <si>
+    <t>Persona  80</t>
+  </si>
+  <si>
+    <t>LONG</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>Persona  81</t>
+  </si>
+  <si>
+    <t>Profile Classification</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Dubai Residence</t>
+  </si>
+  <si>
+    <t>GCC</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>COLORED</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>License Status</t>
+  </si>
+  <si>
+    <t>Declared</t>
+  </si>
+  <si>
+    <t>Proof Ownership</t>
+  </si>
+  <si>
+    <t>Has UAE Fines</t>
+  </si>
+  <si>
+    <t>Persona  82</t>
+  </si>
+  <si>
+    <t>Persona  83</t>
+  </si>
+  <si>
+    <t>1998</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>Has UAE And GCC Fines</t>
+  </si>
+  <si>
+    <t>Has UAE and Salik Fines</t>
+  </si>
+  <si>
+    <t>Persona  84</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>Persona  85</t>
+  </si>
+  <si>
+    <t>MOTORCYCLE</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>Vehicle Decleared</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>InsurancePeriod</t>
+  </si>
+  <si>
+    <t>licensePeriod</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>VCL_ID_1</t>
+  </si>
+  <si>
+    <t>دراجة نارية</t>
+  </si>
+  <si>
+    <t>Motor Cycle</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Persona  01</t>
+  </si>
+  <si>
+    <t>2101</t>
+  </si>
+  <si>
+    <t>مركبة ثقيلة</t>
+  </si>
+  <si>
+    <t>Heavy Vehicle</t>
+  </si>
+  <si>
+    <t>VCL_ID_5</t>
+  </si>
+  <si>
+    <t>Persona Nigative 02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,8 +245,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,8 +272,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -165,35 +302,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -201,13 +314,21 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,131 +609,663 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U2" sqref="A2:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" customWidth="1"/>
+    <col min="18" max="18" width="26" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>26</v>
+      <c r="N1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="M3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="5" t="b">
-        <v>1</v>
+      <c r="P4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{B8797854-1B79-453E-AFD0-995BA4420426}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U8" xr:uid="{B8797854-1B79-453E-AFD0-995BA4420426}">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0F1F1B-D6EF-4868-B6DA-0537089EDB09}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{3F801DFB-5365-4CF4-96FF-29211C89A63B}">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update declare & Register Negative Scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
+++ b/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.afify\IdeaProjects\vls-frontend-automation\src\test\resources\TestDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA52DAE-BD93-4C47-BF94-3F5452346DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AC2B86-00B6-406C-95AF-F28FE36D9F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewVehicleDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="declareVehicleDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="AlternativeDataRegisterVehicle" sheetId="3" r:id="rId2"/>
+    <sheet name="declareVehicleDetails" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="76">
   <si>
     <t>Persona_No</t>
   </si>
@@ -224,6 +225,36 @@
   </si>
   <si>
     <t>Persona Nigative 02</t>
+  </si>
+  <si>
+    <t>Persona Nigative 01</t>
+  </si>
+  <si>
+    <t>Persona Negative 01</t>
+  </si>
+  <si>
+    <t>ScenarioType</t>
+  </si>
+  <si>
+    <t>Persona Negative 02</t>
+  </si>
+  <si>
+    <t>noProfileExist</t>
+  </si>
+  <si>
+    <t>Persona Negative 03</t>
+  </si>
+  <si>
+    <t>noInsurancePolicy</t>
+  </si>
+  <si>
+    <t>2102</t>
+  </si>
+  <si>
+    <t>Persona Negative 04</t>
+  </si>
+  <si>
+    <t>vehicleNoDeclaredNoOwned</t>
   </si>
 </sst>
 </file>
@@ -611,13 +642,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U2" sqref="A2:U2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -766,7 +797,7 @@
         <v>30</v>
       </c>
       <c r="U2" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="17.25" x14ac:dyDescent="0.25">
@@ -1172,11 +1203,236 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D478377-A14A-4795-B3E6-3A7DFAAD32A7}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L5" xr:uid="{96546EC7-9113-4FCF-BD4E-AA1C2917F929}">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0F1F1B-D6EF-4868-B6DA-0537089EDB09}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,7 +1493,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>61</v>
@@ -1255,13 +1511,36 @@
         <v>27</v>
       </c>
       <c r="G3" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{3F801DFB-5365-4CF4-96FF-29211C89A63B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4" xr:uid="{3F801DFB-5365-4CF4-96FF-29211C89A63B}">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update for Vehicle Renewal
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
+++ b/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.afify\IdeaProjects\vls-frontend-automation\src\test\resources\TestDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C42B450-C6BD-45EF-A9D2-6F7BE7109767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F41284-F335-4C48-A2CF-79218C579331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,17 +18,24 @@
     <sheet name="declareVehicleDetails" sheetId="2" r:id="rId3"/>
     <sheet name="vehicleRenewalTestData" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="93">
   <si>
     <t>Persona_No</t>
   </si>
@@ -273,9 +280,6 @@
     <t>3000</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>TestCaseNo</t>
   </si>
   <si>
@@ -288,10 +292,28 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>TRUE</t>
+    <t>FALSE</t>
   </si>
   <si>
     <t>Has UAE And GCC AND SALIK Fines</t>
+  </si>
+  <si>
+    <t>4000</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>TC 002</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>TC 003</t>
+  </si>
+  <si>
+    <t>401</t>
   </si>
 </sst>
 </file>
@@ -1594,10 +1616,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7891A885-86DE-40DD-AFB1-8B71A8E9D7D3}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,7 +1636,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>78</v>
@@ -1635,7 +1657,7 @@
         <v>76</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>24</v>
@@ -1643,13 +1665,13 @@
     </row>
     <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -1658,31 +1680,89 @@
         <v>16</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>84</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{44AEF944-21FC-4E8F-9C8F-E2B04C0CAC21}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I4" xr:uid="{44AEF944-21FC-4E8F-9C8F-E2B04C0CAC21}">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{91ED8A62-B860-4721-B50D-426111C41BBC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4" xr:uid="{91ED8A62-B860-4721-B50D-426111C41BBC}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{4488D1AC-559C-403D-BCDF-8DABB77D463B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{4488D1AC-559C-403D-BCDF-8DABB77D463B}">
       <formula1>"PASSED,FAILED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{B8707C9E-902A-4EC4-BAF4-5FB26A12DE6D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{B8707C9E-902A-4EC4-BAF4-5FB26A12DE6D}">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update for Vehicle Renewal 3
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
+++ b/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.afify\IdeaProjects\vls-frontend-automation\src\test\resources\TestDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F41284-F335-4C48-A2CF-79218C579331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C20830-E57A-446D-8ED8-7247AEA6F742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -313,7 +313,7 @@
     <t>TC 003</t>
   </si>
   <si>
-    <t>401</t>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -1619,7 +1619,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update for Vehicle Renewal & Login For Corporate
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
+++ b/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.afify\IdeaProjects\vls-frontend-automation\src\test\resources\TestDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C20830-E57A-446D-8ED8-7247AEA6F742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB8260F-08A0-45D3-B3BB-EF71B1FB9474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="90">
   <si>
     <t>Persona_No</t>
   </si>
@@ -287,15 +287,6 @@
   </si>
   <si>
     <t>True</t>
-  </si>
-  <si>
-    <t>PASSED</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>Has UAE And GCC AND SALIK Fines</t>
   </si>
   <si>
     <t>4000</t>
@@ -1616,10 +1607,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7891A885-86DE-40DD-AFB1-8B71A8E9D7D3}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,12 +1620,10 @@
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
@@ -1651,19 +1640,13 @@
         <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>82</v>
       </c>
@@ -1671,7 +1654,7 @@
         <v>80</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -1680,27 +1663,21 @@
         <v>16</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>80</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -1709,21 +1686,15 @@
         <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I3" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>79</v>
@@ -1738,34 +1709,23 @@
         <v>16</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" s="8" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I4" xr:uid="{44AEF944-21FC-4E8F-9C8F-E2B04C0CAC21}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4" xr:uid="{44AEF944-21FC-4E8F-9C8F-E2B04C0CAC21}">
       <formula1>"True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4" xr:uid="{91ED8A62-B860-4721-B50D-426111C41BBC}">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{4488D1AC-559C-403D-BCDF-8DABB77D463B}">
-      <formula1>"PASSED,FAILED"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{B8707C9E-902A-4EC4-BAF4-5FB26A12DE6D}">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update for Vehicle Renewal Excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
+++ b/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.afify\IdeaProjects\vls-frontend-automation\src\test\resources\TestDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C642ECBB-30C9-43CF-9C08-98FF0D006F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4500A784-8884-4BA1-96F3-FBFBC05B8FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="vehicleRenewalTestData" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1619,7 +1620,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Vehicle Renewal with Aramex delivery
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
+++ b/src/test/resources/TestDataFiles/NewVehicleDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.afify\IdeaProjects\vls-frontend-automation\src\test\resources\TestDataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\IDrive-Sync\DevOps_Repos\vls-frontend-automation\src\test\resources\TestDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4500A784-8884-4BA1-96F3-FBFBC05B8FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D60A5A-2793-4568-B0AC-0C3E1636B029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewVehicleDetails" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="declareVehicleDetails" sheetId="2" r:id="rId3"/>
     <sheet name="vehicleRenewalTestData" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -275,46 +276,46 @@
     <t>VehicleWeightFrom</t>
   </si>
   <si>
-    <t>1000</t>
+    <t>TestCaseNo</t>
+  </si>
+  <si>
+    <t>TC 001</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>TC 002</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>TC 003</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>3100</t>
+  </si>
+  <si>
+    <t>4000</t>
   </si>
   <si>
     <t>3000</t>
   </si>
   <si>
-    <t>TestCaseNo</t>
-  </si>
-  <si>
-    <t>TC 001</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>4000</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>TC 002</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>TC 003</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>3100</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>4100</t>
+  </si>
+  <si>
+    <t>12000</t>
   </si>
 </sst>
 </file>
@@ -397,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -426,6 +427,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1617,25 +1619,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7891A885-86DE-40DD-AFB1-8B71A8E9D7D3}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>78</v>
@@ -1656,15 +1658,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>90</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -1673,21 +1675,24 @@
         <v>16</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H2">
+        <v>150434394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>92</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -1696,21 +1701,24 @@
         <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H3" s="10">
+        <v>150434851</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -1719,10 +1727,10 @@
         <v>16</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>